<commit_message>
indent code and update WBS
</commit_message>
<xml_diff>
--- a/wbs.xlsx
+++ b/wbs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariel.melaragno/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariel.melaragno/Desktop/Lucky/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99980977-F899-084E-B9CA-C7284D94C946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905AF52F-97F0-B641-AB19-F56D3B2C1C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28220" windowHeight="16460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,14 @@
     <sheet name="WBS Diagram" sheetId="1" r:id="rId1"/>
     <sheet name="WBS Outline" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>DATE</t>
   </si>
@@ -64,58 +70,61 @@
     <t>Analysis</t>
   </si>
   <si>
-    <t>Read the document   (1Hr)</t>
-  </si>
-  <si>
-    <t>Tests endoints.   (1Hr)</t>
-  </si>
-  <si>
-    <t>Submit questions   (1 Hr)</t>
-  </si>
-  <si>
-    <t>Postman tests ( 1Hr)</t>
-  </si>
-  <si>
     <t>Investigation</t>
-  </si>
-  <si>
-    <t>Tools (1Hr)</t>
-  </si>
-  <si>
-    <t>Languages (1 Hr)</t>
-  </si>
-  <si>
-    <t>Apis (2 Hr)</t>
   </si>
   <si>
     <t>Develop</t>
   </si>
   <si>
-    <t>Steps (3 Hr)</t>
-  </si>
-  <si>
-    <t>Test ( 3 Hr)</t>
-  </si>
-  <si>
     <t>Documentation</t>
-  </si>
-  <si>
-    <t>WBS ( 1 Hr)</t>
-  </si>
-  <si>
-    <t>Readme (2 Hr)</t>
-  </si>
-  <si>
-    <t>Configurations ( 6 Hr)</t>
-  </si>
-  <si>
-    <t>Connectors ( 6 Hr)</t>
   </si>
   <si>
     <t>TOTAL 29 hs</t>
   </si>
   <si>
     <t>Mariel melaragno</t>
+  </si>
+  <si>
+    <t>HOURS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read the document  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit questions   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tests endpoints.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postman tests </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Languages </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connectors </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configurations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Readme </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WBS </t>
   </si>
 </sst>
 </file>
@@ -135,16 +144,19 @@
       <sz val="22"/>
       <color theme="4" tint="-0.499984740745262"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -167,34 +179,40 @@
       <sz val="20"/>
       <color theme="4" tint="-0.499984740745262"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -355,7 +373,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -386,9 +404,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -398,10 +413,35 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -425,13 +465,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -441,15 +475,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,22 +494,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -3938,35 +3947,35 @@
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="25">
         <v>44027</v>
       </c>
-      <c r="H4" s="17"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3997,22 +4006,22 @@
     <row r="31" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
     </row>
     <row r="34" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
     </row>
     <row r="35" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4038,10 +4047,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:E44"/>
+  <dimension ref="B1:F44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4051,11 +4060,11 @@
     <col min="3" max="3" width="45" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="24" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" style="2" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
@@ -4063,236 +4072,286 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="2:5" ht="13.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="20" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>29</v>
+      <c r="C4" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="22">
         <v>44027</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="31" t="s">
+    <row r="5" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="7" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="33">
+    <row r="8" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="16">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
+      <c r="C8" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
+      <c r="C9" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="8">
+    <row r="10" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6">
         <v>1.2</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
+      <c r="C10" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="21">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="11" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
+      <c r="C11" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="21">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="12" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7">
         <v>2</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
+      <c r="C12" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="33">
+    <row r="13" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="16">
         <v>2.1</v>
       </c>
-      <c r="C13" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
+      <c r="C13" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="33">
+    <row r="14" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="16">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="33">
+    <row r="15" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="16">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
+      <c r="C15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="7">
         <v>3</v>
       </c>
-      <c r="C16" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
+      <c r="C16" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="33">
+    <row r="17" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="16">
         <v>3.1</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
+      <c r="C17" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="21">
+        <v>2</v>
+      </c>
     </row>
-    <row r="18" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="33">
+    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="16">
         <v>3.2</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="19" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="33">
+    <row r="19" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="16">
         <v>3.3</v>
       </c>
-      <c r="C19" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
+      <c r="C19" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="21">
+        <v>6</v>
+      </c>
     </row>
-    <row r="20" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="8">
         <v>4</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
+      <c r="C20" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="21">
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="8">
         <v>5</v>
       </c>
-      <c r="C21" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
+      <c r="C21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="21"/>
     </row>
-    <row r="22" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="40">
+    <row r="22" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="17">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C22" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
+      <c r="C22" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="40">
+    <row r="23" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="17">
         <v>5.2</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="17"/>
+      <c r="C24" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="21">
+        <f>SUM(F7:F23)</f>
         <v>24</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
     </row>
-    <row r="24" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="40"/>
-      <c r="C24" s="42" t="s">
-        <v>28</v>
-      </c>
+    <row r="25" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
-    <row r="25" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+    <row r="26" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
     </row>
-    <row r="26" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4306,22 +4365,22 @@
     <row r="44" ht="22.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>